<commit_message>
load balancing; TODO samples vs acc, error bars, server vs time rework
</commit_message>
<xml_diff>
--- a/ml/results/servers=13_vs_time_success=0.90.xlsx
+++ b/ml/results/servers=13_vs_time_success=0.90.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Zachary/Desktop/Research/projects/mimosa_2022/MIMOSA/ml/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04D707AC-C590-4F43-B12D-E442E4FC243B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF30A4BD-BB48-3A40-8B60-3D21F5A99D64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25900" windowHeight="15280" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19480" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="wrr" sheetId="1" r:id="rId1"/>
+    <sheet name="ideal" sheetId="1" r:id="rId1"/>
     <sheet name="random" sheetId="2" r:id="rId2"/>
     <sheet name="koth" sheetId="3" r:id="rId3"/>
     <sheet name="mimosa" sheetId="4" r:id="rId4"/>
@@ -128,31 +128,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t># of Servers vs Runtime</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -207,7 +182,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>random!$B$2:$B$14</c:f>
+              <c:f>mimosa!$B$2:$B$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -255,7 +230,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>wrr!$D$2:$D$14</c:f>
+              <c:f>ideal!$D$2:$D$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -281,29 +256,29 @@
                   <c:v>37534.300000000003</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>37534.300000000003</c:v>
+                  <c:v>35874.9</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>37534.300000000003</c:v>
+                  <c:v>34928.699999999997</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>37534.300000000003</c:v>
+                  <c:v>30004.099999999991</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>37534.300000000003</c:v>
+                  <c:v>27837.200000000001</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>37534.300000000003</c:v>
+                  <c:v>19199.900000000001</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>37534.300000000003</c:v>
+                  <c:v>18334.400000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-D371-1C40-83A5-90FB85EAA10F}"/>
+              <c16:uniqueId val="{00000000-1CDB-9B42-9B83-11833D94B8F2}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -325,7 +300,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>random!$B$2:$B$14</c:f>
+              <c:f>mimosa!$B$2:$B$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -378,50 +353,50 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
                 <c:pt idx="0">
-                  <c:v>270098.90000000002</c:v>
+                  <c:v>321291.40000000008</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>141587.5</c:v>
+                  <c:v>166168.4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>103823.2</c:v>
+                  <c:v>119806.39999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>80819</c:v>
+                  <c:v>91285.7</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>68804.600000000006</c:v>
+                  <c:v>80672.3</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>68160</c:v>
+                  <c:v>76767.400000000009</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>63647.8</c:v>
+                  <c:v>71123.900000000009</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>49363.3</c:v>
+                  <c:v>77834.900000000009</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>46884.7</c:v>
+                  <c:v>71585.500000000015</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>59780.2</c:v>
+                  <c:v>77739.000000000015</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>71383</c:v>
+                  <c:v>71662.399999999994</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>61714</c:v>
+                  <c:v>54093</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>65581.600000000006</c:v>
+                  <c:v>64582</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-D371-1C40-83A5-90FB85EAA10F}"/>
+              <c16:uniqueId val="{00000001-1CDB-9B42-9B83-11833D94B8F2}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -443,7 +418,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>random!$B$2:$B$14</c:f>
+              <c:f>mimosa!$B$2:$B$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -496,50 +471,50 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
                 <c:pt idx="0">
-                  <c:v>90190.900000000009</c:v>
+                  <c:v>112226.3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>90190.900000000009</c:v>
+                  <c:v>55606.499999999993</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>90190.900000000009</c:v>
+                  <c:v>50743.9</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>90190.900000000009</c:v>
+                  <c:v>26664.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>90190.900000000009</c:v>
+                  <c:v>27943.9</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>90190.900000000009</c:v>
+                  <c:v>27673.7</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>90190.900000000009</c:v>
+                  <c:v>26754.900000000009</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>90190.900000000009</c:v>
+                  <c:v>14583.7</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>90190.900000000009</c:v>
+                  <c:v>14583.7</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>90190.900000000009</c:v>
+                  <c:v>13623.3</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>90190.900000000009</c:v>
+                  <c:v>14340.5</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>90190.900000000009</c:v>
+                  <c:v>14173.9</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>90190.900000000009</c:v>
+                  <c:v>14398.9</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-D371-1C40-83A5-90FB85EAA10F}"/>
+              <c16:uniqueId val="{00000002-1CDB-9B42-9B83-11833D94B8F2}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -561,7 +536,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>random!$B$2:$B$14</c:f>
+              <c:f>mimosa!$B$2:$B$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -614,50 +589,50 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
                 <c:pt idx="0">
-                  <c:v>199161.5</c:v>
+                  <c:v>200544</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>114198.8</c:v>
+                  <c:v>115182.3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>77013.899999999994</c:v>
+                  <c:v>75524.7</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>70343.3</c:v>
+                  <c:v>69791</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>49861.599999999999</c:v>
+                  <c:v>48201.9</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>45526.899999999987</c:v>
+                  <c:v>44470.399999999987</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>46173.2</c:v>
+                  <c:v>48643.199999999997</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>47661</c:v>
+                  <c:v>40997.1</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>44176.3</c:v>
+                  <c:v>41058.399999999987</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>46468.1</c:v>
+                  <c:v>34802.699999999997</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>44503.7</c:v>
+                  <c:v>31675.900000000009</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>45518.399999999987</c:v>
+                  <c:v>22972.9</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>45158.499999999993</c:v>
+                  <c:v>22357.200000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-D371-1C40-83A5-90FB85EAA10F}"/>
+              <c16:uniqueId val="{00000003-1CDB-9B42-9B83-11833D94B8F2}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -671,71 +646,16 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="326300096"/>
-        <c:axId val="326156176"/>
+        <c:axId val="1064750656"/>
+        <c:axId val="1064608368"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="326300096"/>
+        <c:axId val="1064750656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t># of Servers</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -773,7 +693,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="326156176"/>
+        <c:crossAx val="1064608368"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -781,7 +701,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="326156176"/>
+        <c:axId val="1064608368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -801,61 +721,6 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Runtime</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -887,7 +752,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="326300096"/>
+        <c:crossAx val="1064750656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1521,23 +1386,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>723900</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>82550</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>419100</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>165100</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>425450</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>146050</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{07691934-0032-90EE-6E08-3E25DADAFEE2}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9C7742D0-7850-16EA-8551-A9B731681F72}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1990,10 +1855,10 @@
         <v>8</v>
       </c>
       <c r="C9">
-        <v>0.87424575332491594</v>
+        <v>0.87424575332491616</v>
       </c>
       <c r="D9">
-        <v>37534.300000000003</v>
+        <v>35874.9</v>
       </c>
       <c r="E9">
         <v>1</v>
@@ -2010,7 +1875,7 @@
         <v>0.87424575332491594</v>
       </c>
       <c r="D10">
-        <v>37534.300000000003</v>
+        <v>34928.699999999997</v>
       </c>
       <c r="E10">
         <v>1</v>
@@ -2027,7 +1892,7 @@
         <v>0.87424575332491594</v>
       </c>
       <c r="D11">
-        <v>37534.300000000003</v>
+        <v>30004.099999999991</v>
       </c>
       <c r="E11">
         <v>1</v>
@@ -2044,7 +1909,7 @@
         <v>0.87424575332491594</v>
       </c>
       <c r="D12">
-        <v>37534.300000000003</v>
+        <v>27837.200000000001</v>
       </c>
       <c r="E12">
         <v>1</v>
@@ -2061,7 +1926,7 @@
         <v>0.87424575332491594</v>
       </c>
       <c r="D13">
-        <v>37534.300000000003</v>
+        <v>19199.900000000001</v>
       </c>
       <c r="E13">
         <v>1</v>
@@ -2075,10 +1940,10 @@
         <v>13</v>
       </c>
       <c r="C14">
-        <v>0.87424575332491594</v>
+        <v>0.87424575332491572</v>
       </c>
       <c r="D14">
-        <v>37534.300000000003</v>
+        <v>18334.400000000001</v>
       </c>
       <c r="E14">
         <v>1</v>
@@ -2119,13 +1984,13 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>0.54174204782538027</v>
+        <v>0.62662322961736949</v>
       </c>
       <c r="D2">
-        <v>270098.90000000002</v>
+        <v>321291.40000000008</v>
       </c>
       <c r="E2">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -2136,13 +2001,13 @@
         <v>2</v>
       </c>
       <c r="C3">
-        <v>0.54289800648512676</v>
+        <v>0.50424252089723576</v>
       </c>
       <c r="D3">
-        <v>141587.5</v>
+        <v>166168.4</v>
       </c>
       <c r="E3">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -2153,13 +2018,13 @@
         <v>3</v>
       </c>
       <c r="C4">
-        <v>0.55423986048480789</v>
+        <v>0.46550020356613953</v>
       </c>
       <c r="D4">
-        <v>103823.2</v>
+        <v>119806.39999999999</v>
       </c>
       <c r="E4">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -2170,13 +2035,13 @@
         <v>4</v>
       </c>
       <c r="C5">
-        <v>0.54618278832852818</v>
+        <v>0.55968554946365778</v>
       </c>
       <c r="D5">
-        <v>80819</v>
+        <v>91285.7</v>
       </c>
       <c r="E5">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -2187,13 +2052,13 @@
         <v>5</v>
       </c>
       <c r="C6">
-        <v>0.53478038338508249</v>
+        <v>0.3856163506262949</v>
       </c>
       <c r="D6">
-        <v>68804.600000000006</v>
+        <v>80672.3</v>
       </c>
       <c r="E6">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -2204,13 +2069,13 @@
         <v>6</v>
       </c>
       <c r="C7">
-        <v>0.55674906981729355</v>
+        <v>0.55893389273246041</v>
       </c>
       <c r="D7">
-        <v>68160</v>
+        <v>76767.400000000009</v>
       </c>
       <c r="E7">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -2221,13 +2086,13 @@
         <v>7</v>
       </c>
       <c r="C8">
-        <v>0.5503954174892699</v>
+        <v>0.38248587333914491</v>
       </c>
       <c r="D8">
-        <v>63647.8</v>
+        <v>71123.900000000009</v>
       </c>
       <c r="E8">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -2238,13 +2103,13 @@
         <v>8</v>
       </c>
       <c r="C9">
-        <v>0.55385661155675392</v>
+        <v>0.41308130458302678</v>
       </c>
       <c r="D9">
-        <v>49363.3</v>
+        <v>77834.900000000009</v>
       </c>
       <c r="E9">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
@@ -2255,13 +2120,13 @@
         <v>9</v>
       </c>
       <c r="C10">
-        <v>0.55658730273874057</v>
+        <v>0.51427557676233882</v>
       </c>
       <c r="D10">
-        <v>46884.7</v>
+        <v>71585.500000000015</v>
       </c>
       <c r="E10">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
@@ -2272,13 +2137,13 @@
         <v>10</v>
       </c>
       <c r="C11">
-        <v>0.53821022779119043</v>
+        <v>0.59243895877620634</v>
       </c>
       <c r="D11">
-        <v>59780.2</v>
+        <v>77739.000000000015</v>
       </c>
       <c r="E11">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -2289,13 +2154,13 @@
         <v>11</v>
       </c>
       <c r="C12">
-        <v>0.52623320104820126</v>
+        <v>0.40163603058931269</v>
       </c>
       <c r="D12">
-        <v>71383</v>
+        <v>71662.399999999994</v>
       </c>
       <c r="E12">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
@@ -2306,13 +2171,13 @@
         <v>12</v>
       </c>
       <c r="C13">
-        <v>0.53809273105523303</v>
+        <v>0.6032297137990047</v>
       </c>
       <c r="D13">
-        <v>61714</v>
+        <v>54093</v>
       </c>
       <c r="E13">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
@@ -2323,13 +2188,13 @@
         <v>13</v>
       </c>
       <c r="C14">
-        <v>0.5494468850588512</v>
+        <v>0.42280711214378069</v>
       </c>
       <c r="D14">
-        <v>65581.600000000006</v>
+        <v>64582</v>
       </c>
       <c r="E14">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -2367,13 +2232,13 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>0.83992808894685067</v>
+        <v>0.87169363717700554</v>
       </c>
       <c r="D2">
-        <v>90190.900000000009</v>
+        <v>112226.3</v>
       </c>
       <c r="E2">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -2384,13 +2249,13 @@
         <v>2</v>
       </c>
       <c r="C3">
-        <v>0.83992808894685067</v>
+        <v>0.86794451315928611</v>
       </c>
       <c r="D3">
-        <v>90190.900000000009</v>
+        <v>55606.499999999993</v>
       </c>
       <c r="E3">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -2401,13 +2266,13 @@
         <v>3</v>
       </c>
       <c r="C4">
-        <v>0.83992808894685067</v>
+        <v>0.79660195747746776</v>
       </c>
       <c r="D4">
-        <v>90190.900000000009</v>
+        <v>50743.9</v>
       </c>
       <c r="E4">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -2418,13 +2283,13 @@
         <v>4</v>
       </c>
       <c r="C5">
-        <v>0.83992808894685067</v>
+        <v>0.74214758676560355</v>
       </c>
       <c r="D5">
-        <v>90190.900000000009</v>
+        <v>26664.5</v>
       </c>
       <c r="E5">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -2435,13 +2300,13 @@
         <v>5</v>
       </c>
       <c r="C6">
-        <v>0.83992808894685067</v>
+        <v>0.81343258723087153</v>
       </c>
       <c r="D6">
-        <v>90190.900000000009</v>
+        <v>27943.9</v>
       </c>
       <c r="E6">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -2452,13 +2317,13 @@
         <v>6</v>
       </c>
       <c r="C7">
-        <v>0.83992808894685067</v>
+        <v>0.87925896993625063</v>
       </c>
       <c r="D7">
-        <v>90190.900000000009</v>
+        <v>27673.7</v>
       </c>
       <c r="E7">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -2469,13 +2334,13 @@
         <v>7</v>
       </c>
       <c r="C8">
-        <v>0.83992808894685067</v>
+        <v>0.86732640881028766</v>
       </c>
       <c r="D8">
-        <v>90190.900000000009</v>
+        <v>26754.900000000009</v>
       </c>
       <c r="E8">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -2486,13 +2351,13 @@
         <v>8</v>
       </c>
       <c r="C9">
-        <v>0.83992808894685067</v>
+        <v>0.80568418153595633</v>
       </c>
       <c r="D9">
-        <v>90190.900000000009</v>
+        <v>14583.7</v>
       </c>
       <c r="E9">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
@@ -2503,13 +2368,13 @@
         <v>9</v>
       </c>
       <c r="C10">
-        <v>0.83992808894685067</v>
+        <v>0.81980507766589972</v>
       </c>
       <c r="D10">
-        <v>90190.900000000009</v>
+        <v>14583.7</v>
       </c>
       <c r="E10">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
@@ -2520,13 +2385,13 @@
         <v>10</v>
       </c>
       <c r="C11">
-        <v>0.83992808894685067</v>
+        <v>0.82315578149640833</v>
       </c>
       <c r="D11">
-        <v>90190.900000000009</v>
+        <v>13623.3</v>
       </c>
       <c r="E11">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -2537,13 +2402,13 @@
         <v>11</v>
       </c>
       <c r="C12">
-        <v>0.83992808894685067</v>
+        <v>0.78439966295705199</v>
       </c>
       <c r="D12">
-        <v>90190.900000000009</v>
+        <v>14340.5</v>
       </c>
       <c r="E12">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
@@ -2554,13 +2419,13 @@
         <v>12</v>
       </c>
       <c r="C13">
-        <v>0.83992808894685067</v>
+        <v>0.76261703780149315</v>
       </c>
       <c r="D13">
-        <v>90190.900000000009</v>
+        <v>14173.9</v>
       </c>
       <c r="E13">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
@@ -2571,13 +2436,13 @@
         <v>13</v>
       </c>
       <c r="C14">
-        <v>0.83992808894685067</v>
+        <v>0.85944796295968517</v>
       </c>
       <c r="D14">
-        <v>90190.900000000009</v>
+        <v>14398.9</v>
       </c>
       <c r="E14">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -2615,10 +2480,10 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>0.88564327019087408</v>
+        <v>0.86710041854657705</v>
       </c>
       <c r="D2">
-        <v>199161.5</v>
+        <v>200544</v>
       </c>
       <c r="E2">
         <v>3</v>
@@ -2632,10 +2497,10 @@
         <v>2</v>
       </c>
       <c r="C3">
-        <v>0.86601052668063228</v>
+        <v>0.87983768880527491</v>
       </c>
       <c r="D3">
-        <v>114198.8</v>
+        <v>115182.3</v>
       </c>
       <c r="E3">
         <v>3</v>
@@ -2649,10 +2514,10 @@
         <v>3</v>
       </c>
       <c r="C4">
-        <v>0.88443542298709321</v>
+        <v>0.833963206919626</v>
       </c>
       <c r="D4">
-        <v>77013.899999999994</v>
+        <v>75524.7</v>
       </c>
       <c r="E4">
         <v>3</v>
@@ -2666,13 +2531,13 @@
         <v>4</v>
       </c>
       <c r="C5">
-        <v>0.88155288709249036</v>
+        <v>0.87066769686756462</v>
       </c>
       <c r="D5">
-        <v>70343.3</v>
+        <v>69791</v>
       </c>
       <c r="E5">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -2683,10 +2548,10 @@
         <v>5</v>
       </c>
       <c r="C6">
-        <v>0.83622525197369002</v>
+        <v>0.87393086273447362</v>
       </c>
       <c r="D6">
-        <v>49861.599999999999</v>
+        <v>48201.9</v>
       </c>
       <c r="E6">
         <v>3</v>
@@ -2700,10 +2565,10 @@
         <v>6</v>
       </c>
       <c r="C7">
-        <v>0.86221209013975175</v>
+        <v>0.87249194529012364</v>
       </c>
       <c r="D7">
-        <v>45526.899999999987</v>
+        <v>44470.399999999987</v>
       </c>
       <c r="E7">
         <v>3</v>
@@ -2717,13 +2582,13 @@
         <v>7</v>
       </c>
       <c r="C8">
-        <v>0.87082130548484871</v>
+        <v>0.89374168954335009</v>
       </c>
       <c r="D8">
-        <v>46173.2</v>
+        <v>48643.199999999997</v>
       </c>
       <c r="E8">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -2734,13 +2599,13 @@
         <v>8</v>
       </c>
       <c r="C9">
-        <v>0.88840562330051642</v>
+        <v>0.88032679301571282</v>
       </c>
       <c r="D9">
-        <v>47661</v>
+        <v>40997.1</v>
       </c>
       <c r="E9">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
@@ -2751,13 +2616,13 @@
         <v>9</v>
       </c>
       <c r="C10">
-        <v>0.8395366314416387</v>
+        <v>0.86545796667889485</v>
       </c>
       <c r="D10">
-        <v>44176.3</v>
+        <v>41058.399999999987</v>
       </c>
       <c r="E10">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
@@ -2768,13 +2633,13 @@
         <v>10</v>
       </c>
       <c r="C11">
-        <v>0.86685376870332087</v>
+        <v>0.90939243667684744</v>
       </c>
       <c r="D11">
-        <v>46468.1</v>
+        <v>34802.699999999997</v>
       </c>
       <c r="E11">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -2785,10 +2650,10 @@
         <v>11</v>
       </c>
       <c r="C12">
-        <v>0.87561109990460162</v>
+        <v>0.8733073371689114</v>
       </c>
       <c r="D12">
-        <v>44503.7</v>
+        <v>31675.900000000009</v>
       </c>
       <c r="E12">
         <v>3</v>
@@ -2802,10 +2667,10 @@
         <v>12</v>
       </c>
       <c r="C13">
-        <v>0.89463897516891144</v>
+        <v>0.87833513223010018</v>
       </c>
       <c r="D13">
-        <v>45518.399999999987</v>
+        <v>22972.9</v>
       </c>
       <c r="E13">
         <v>3</v>
@@ -2819,10 +2684,10 @@
         <v>13</v>
       </c>
       <c r="C14">
-        <v>0.86109800603052744</v>
+        <v>0.84959296920549343</v>
       </c>
       <c r="D14">
-        <v>45158.499999999993</v>
+        <v>22357.200000000001</v>
       </c>
       <c r="E14">
         <v>3</v>
@@ -2834,7 +2699,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA8D5567-3C4A-1C43-AA5F-B756B0FDA0DD}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B1AC265-F309-6F44-90AE-81FCC389CC9D}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>